<commit_message>
Fixed IceWall string in Card Library so card loads properly
</commit_message>
<xml_diff>
--- a/data/SBCCG_Card_Library.xlsx
+++ b/data/SBCCG_Card_Library.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="408">
   <si>
     <t>LongName</t>
   </si>
@@ -1243,9 +1243,6 @@
   </si>
   <si>
     <t>Error</t>
-  </si>
-  <si>
-    <t>Ice Wall</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11"/>
+      <selection pane="topRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>408</v>
+        <v>348</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">

</xml_diff>

<commit_message>
Sprint and Rest are no longer repeatable, no longer required cards
</commit_message>
<xml_diff>
--- a/data/SBCCG_Card_Library.xlsx
+++ b/data/SBCCG_Card_Library.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="407">
   <si>
     <t>LongName</t>
   </si>
@@ -1011,12 +1011,6 @@
     <t>Skill</t>
   </si>
   <si>
-    <t>Pay 4: Draw a card.  Repeatable</t>
-  </si>
-  <si>
-    <t>Star Repeatable</t>
-  </si>
-  <si>
     <t>rest_by_oscarsnapshotter_d16yiqm.jpg</t>
   </si>
   <si>
@@ -1221,9 +1215,6 @@
     <t xml:space="preserve">When a friendly minion dies, summon this from your deck.  </t>
   </si>
   <si>
-    <t>Discard a card to gain 1 mana. Repeatable</t>
-  </si>
-  <si>
     <t>Star Hidden</t>
   </si>
   <si>
@@ -1243,6 +1234,12 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>Pay 4: Draw a card</t>
+  </si>
+  <si>
+    <t>Discard a card to gain 1 mana</t>
   </si>
 </sst>
 </file>
@@ -2116,8 +2113,8 @@
   <dimension ref="A1:U137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,7 +2258,7 @@
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2330,10 +2327,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>330</v>
+        <v>405</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -2346,10 +2343,10 @@
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2">
@@ -2359,11 +2356,11 @@
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>130</v>
@@ -2381,10 +2378,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="M5" s="2">
         <v>0</v>
@@ -2397,10 +2394,10 @@
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2">
@@ -2410,11 +2407,11 @@
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>22</v>
@@ -2626,17 +2623,17 @@
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F10" s="5">
         <v>1</v>
@@ -2652,7 +2649,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5">
@@ -2705,7 +2702,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2">
@@ -2736,7 +2733,7 @@
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>40</v>
@@ -2840,11 +2837,11 @@
     </row>
     <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>78</v>
@@ -2891,16 +2888,16 @@
     </row>
     <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F15" s="5">
         <v>2</v>
@@ -2915,7 +2912,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="M15" s="5">
         <v>0</v>
@@ -3254,7 +3251,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>130</v>
@@ -3682,7 +3679,7 @@
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>22</v>
@@ -3986,7 +3983,7 @@
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>22</v>
@@ -4412,7 +4409,7 @@
         <v>4</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="M44" s="2">
         <v>1</v>
@@ -4438,7 +4435,7 @@
         <v>163</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>130</v>
@@ -4845,7 +4842,7 @@
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>78</v>
@@ -4941,11 +4938,11 @@
     </row>
     <row r="55" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>78</v>
@@ -4969,7 +4966,7 @@
         <v>5</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1">
@@ -4994,11 +4991,11 @@
     </row>
     <row r="56" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>78</v>
@@ -5016,7 +5013,7 @@
         <v>5</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1">
@@ -5029,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="Q56" s="1"/>
       <c r="R56" s="1" t="s">
@@ -5043,11 +5040,11 @@
     </row>
     <row r="57" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>78</v>
@@ -5067,7 +5064,7 @@
         <v>5</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1">
@@ -5098,7 +5095,7 @@
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>56</v>
@@ -5145,11 +5142,11 @@
     </row>
     <row r="59" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>56</v>
@@ -5171,7 +5168,7 @@
         <v>6</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="5">
@@ -5208,7 +5205,7 @@
         <v>56</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F60" s="5">
         <v>3</v>
@@ -5244,22 +5241,22 @@
         <v>0</v>
       </c>
       <c r="U60" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F61" s="5">
         <v>5</v>
@@ -5275,7 +5272,7 @@
         <v>4</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="5">
@@ -5297,7 +5294,7 @@
         <v>0</v>
       </c>
       <c r="U61" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -5323,7 +5320,7 @@
         <v>5</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M62" s="9">
         <v>0</v>
@@ -5384,10 +5381,10 @@
     </row>
     <row r="64" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>53</v>
@@ -5402,7 +5399,7 @@
         <v>5</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M64" s="6">
         <v>0</v>
@@ -5422,10 +5419,10 @@
     </row>
     <row r="65" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>53</v>
@@ -5440,7 +5437,7 @@
         <v>5</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M65" s="6">
         <v>0</v>
@@ -5460,10 +5457,10 @@
     </row>
     <row r="66" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>53</v>
@@ -5478,7 +5475,7 @@
         <v>5</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M66" s="6">
         <v>0</v>
@@ -5498,16 +5495,16 @@
     </row>
     <row r="67" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F67" s="6">
         <v>2</v>
@@ -5522,7 +5519,7 @@
         <v>5</v>
       </c>
       <c r="K67" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M67" s="6">
         <v>0</v>
@@ -5534,7 +5531,7 @@
         <v>1</v>
       </c>
       <c r="Q67" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="R67" s="6" t="s">
         <v>27</v>
@@ -5543,21 +5540,21 @@
         <v>0</v>
       </c>
       <c r="U67" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F68" s="6">
         <v>4</v>
@@ -5572,7 +5569,7 @@
         <v>5</v>
       </c>
       <c r="K68" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="M68" s="6">
         <v>0</v>
@@ -5584,7 +5581,7 @@
         <v>1</v>
       </c>
       <c r="Q68" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="R68" s="6" t="s">
         <v>27</v>
@@ -5593,7 +5590,7 @@
         <v>1</v>
       </c>
       <c r="U68" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="69" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -5602,7 +5599,7 @@
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>197</v>
@@ -5649,11 +5646,11 @@
     </row>
     <row r="70" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>197</v>
@@ -5671,7 +5668,7 @@
         <v>5</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L70" s="8"/>
       <c r="M70" s="8">
@@ -5906,7 +5903,7 @@
     </row>
     <row r="75" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="5" t="s">
@@ -5932,7 +5929,7 @@
         <v>6</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L75" s="5"/>
       <c r="M75" s="5">
@@ -6040,7 +6037,7 @@
         <v>6</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L77" s="5"/>
       <c r="M77" s="5">
@@ -6228,7 +6225,7 @@
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>130</v>
@@ -6281,7 +6278,7 @@
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>130</v>
@@ -6842,7 +6839,7 @@
         <v>8</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L93" s="9"/>
       <c r="M93" s="9">
@@ -6895,7 +6892,7 @@
         <v>6</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L94" s="9"/>
       <c r="M94" s="9">
@@ -7395,7 +7392,7 @@
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>130</v>
@@ -7501,7 +7498,7 @@
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>53</v>
@@ -7811,7 +7808,7 @@
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>56</v>
@@ -8021,7 +8018,7 @@
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>130</v>
@@ -8074,7 +8071,7 @@
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>130</v>
@@ -8449,10 +8446,10 @@
         <v>7</v>
       </c>
       <c r="K124" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L124" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M124" s="10">
         <v>1</v>
@@ -8475,10 +8472,10 @@
     </row>
     <row r="125" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D125" s="10" t="s">
         <v>33</v>
@@ -8496,7 +8493,7 @@
         <v>8</v>
       </c>
       <c r="K125" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M125" s="10">
         <v>0</v>
@@ -8520,7 +8517,7 @@
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>78</v>
@@ -8569,11 +8566,11 @@
     </row>
     <row r="127" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>78</v>
@@ -8593,7 +8590,7 @@
         <v>10</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L127" s="1"/>
       <c r="M127" s="1">
@@ -8620,11 +8617,11 @@
     </row>
     <row r="128" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B128" s="5"/>
       <c r="C128" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>56</v>
@@ -8642,7 +8639,7 @@
         <v>10</v>
       </c>
       <c r="K128" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L128" s="5" t="s">
         <v>326</v>
@@ -8669,11 +8666,11 @@
     </row>
     <row r="129" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>197</v>
@@ -8757,7 +8754,7 @@
         <v>0</v>
       </c>
       <c r="P130" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="Q130" s="6" t="s">
         <v>257</v>
@@ -8799,7 +8796,7 @@
         <v>8</v>
       </c>
       <c r="K131" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L131" s="7"/>
       <c r="M131" s="7">
@@ -8826,11 +8823,11 @@
     </row>
     <row r="132" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>78</v>
@@ -8850,7 +8847,7 @@
         <v>15</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>326</v>
@@ -8877,11 +8874,11 @@
     </row>
     <row r="133" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B133" s="5"/>
       <c r="C133" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>56</v>
@@ -8899,7 +8896,7 @@
         <v>15</v>
       </c>
       <c r="K133" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L133" s="5" t="s">
         <v>326</v>
@@ -8926,10 +8923,10 @@
     </row>
     <row r="134" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C134" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>33</v>
@@ -8947,7 +8944,7 @@
         <v>30</v>
       </c>
       <c r="K134" s="10" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L134" s="10" t="s">
         <v>326</v>
@@ -8970,16 +8967,16 @@
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C135" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D135" t="s">
         <v>130</v>
       </c>
       <c r="E135" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F135">
         <v>0</v>
@@ -8994,7 +8991,7 @@
         <v>325</v>
       </c>
       <c r="L135" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M135">
         <v>0</v>
@@ -9014,16 +9011,16 @@
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C136" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D136" t="s">
         <v>130</v>
       </c>
       <c r="E136" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F136">
         <v>0</v>
@@ -9035,10 +9032,10 @@
         <v>10</v>
       </c>
       <c r="K136" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="L136" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M136">
         <v>0</v>
@@ -9058,7 +9055,7 @@
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D137" t="s">
         <v>130</v>
@@ -9073,7 +9070,7 @@
         <v>0</v>
       </c>
       <c r="K137" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="M137">
         <v>0</v>

</xml_diff>

<commit_message>
Added "set" card attribute, which will determine which cards are available for viewing
</commit_message>
<xml_diff>
--- a/data/SBCCG_Card_Library.xlsx
+++ b/data/SBCCG_Card_Library.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="408">
   <si>
     <t>LongName</t>
   </si>
@@ -1240,6 +1240,9 @@
   </si>
   <si>
     <t>Discard a card to gain 1 mana</t>
+  </si>
+  <si>
+    <t>Set</t>
   </si>
 </sst>
 </file>
@@ -2110,11 +2113,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U137"/>
+  <dimension ref="A1:V137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="topRight" activeCell="R134" sqref="R134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2135,14 +2138,15 @@
     <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="55.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" customWidth="1"/>
+    <col min="18" max="18" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2192,22 +2196,25 @@
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>212</v>
       </c>
@@ -2244,19 +2251,22 @@
         <v>0</v>
       </c>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="5">
+        <v>5</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5"/>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5">
+        <v>0</v>
+      </c>
+      <c r="V2" s="5"/>
+    </row>
+    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>362</v>
       </c>
@@ -2294,16 +2304,17 @@
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="5"/>
+      <c r="S3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T3" s="5"/>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>328</v>
       </c>
@@ -2342,19 +2353,22 @@
         <v>4</v>
       </c>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>331</v>
       </c>
@@ -2393,19 +2407,22 @@
         <v>0</v>
       </c>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="2">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>385</v>
       </c>
@@ -2444,19 +2461,22 @@
         <v>0</v>
       </c>
       <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q6" s="9">
+        <v>1</v>
+      </c>
+      <c r="R6" s="9"/>
       <c r="S6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="T6" s="9">
-        <v>0</v>
-      </c>
-      <c r="U6" s="9"/>
-    </row>
-    <row r="7" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U6" s="9">
+        <v>0</v>
+      </c>
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>187</v>
       </c>
@@ -2499,19 +2519,22 @@
         <v>0</v>
       </c>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>221</v>
       </c>
@@ -2554,21 +2577,24 @@
         <v>0</v>
       </c>
       <c r="P8" s="7"/>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="7">
+        <v>2</v>
+      </c>
+      <c r="R8" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="R8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7">
-        <v>0</v>
-      </c>
-      <c r="U8" s="7" t="s">
+      <c r="S8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7">
+        <v>0</v>
+      </c>
+      <c r="V8" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
@@ -2607,21 +2633,24 @@
         <v>0</v>
       </c>
       <c r="P9" s="10"/>
-      <c r="Q9" s="10" t="s">
+      <c r="Q9" s="10">
+        <v>2</v>
+      </c>
+      <c r="R9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10">
-        <v>0</v>
-      </c>
-      <c r="U9" s="10" t="s">
+      <c r="S9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10">
+        <v>0</v>
+      </c>
+      <c r="V9" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>346</v>
       </c>
@@ -2662,19 +2691,22 @@
         <v>0</v>
       </c>
       <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5" t="s">
+      <c r="Q10" s="5">
+        <v>1</v>
+      </c>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>154</v>
       </c>
@@ -2715,19 +2747,22 @@
         <v>0</v>
       </c>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="2">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2">
-        <v>0</v>
-      </c>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>95</v>
       </c>
@@ -2764,23 +2799,26 @@
         <v>0</v>
       </c>
       <c r="P12" s="7"/>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" s="7">
+        <v>3</v>
+      </c>
+      <c r="R12" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="R12" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="S12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="T12" s="7">
-        <v>0</v>
-      </c>
-      <c r="U12" s="7" t="s">
+      <c r="U12" s="7">
+        <v>0</v>
+      </c>
+      <c r="V12" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>190</v>
       </c>
@@ -2821,21 +2859,22 @@
         <v>0</v>
       </c>
       <c r="P13" s="10"/>
-      <c r="Q13" s="10" t="s">
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="R13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10">
-        <v>0</v>
-      </c>
-      <c r="U13" s="10" t="s">
+      <c r="S13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10">
+        <v>0</v>
+      </c>
+      <c r="V13" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>380</v>
       </c>
@@ -2875,18 +2914,19 @@
       </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="R14" s="1"/>
       <c r="S14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="T14" s="1">
-        <v>0</v>
-      </c>
-      <c r="U14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U14" s="1">
+        <v>0</v>
+      </c>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>344</v>
       </c>
@@ -2923,17 +2963,17 @@
       <c r="O15" s="5">
         <v>0</v>
       </c>
-      <c r="R15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="T15" s="5">
-        <v>0</v>
-      </c>
-      <c r="U15" s="5" t="s">
+      <c r="S15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
+      <c r="V15" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -2974,19 +3014,20 @@
         <v>0</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1"/>
-    </row>
-    <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1">
+        <v>0</v>
+      </c>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>249</v>
       </c>
@@ -3027,19 +3068,20 @@
         <v>0</v>
       </c>
       <c r="P17" s="1"/>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="R17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1">
-        <v>0</v>
-      </c>
-      <c r="U17" s="1"/>
-    </row>
-    <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1">
+        <v>0</v>
+      </c>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>262</v>
       </c>
@@ -3080,19 +3122,20 @@
         <v>0</v>
       </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="R18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1">
-        <v>0</v>
-      </c>
-      <c r="U18" s="1"/>
-    </row>
-    <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1">
+        <v>0</v>
+      </c>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>265</v>
       </c>
@@ -3133,21 +3176,22 @@
         <v>0</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="R19" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="S19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T19" s="1">
-        <v>0</v>
-      </c>
-      <c r="U19" s="1"/>
-    </row>
-    <row r="20" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>271</v>
       </c>
@@ -3184,19 +3228,20 @@
         <v>0</v>
       </c>
       <c r="P20" s="1"/>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="R20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1">
-        <v>0</v>
-      </c>
-      <c r="U20" s="1"/>
-    </row>
-    <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>273</v>
       </c>
@@ -3236,16 +3281,17 @@
       </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1">
-        <v>0</v>
-      </c>
-      <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R21" s="1"/>
+      <c r="S21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>129</v>
       </c>
@@ -3288,19 +3334,20 @@
         <v>0</v>
       </c>
       <c r="P22" s="2"/>
-      <c r="Q22" s="2" t="s">
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="R22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2">
-        <v>0</v>
-      </c>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>52</v>
       </c>
@@ -3337,19 +3384,20 @@
         <v>0</v>
       </c>
       <c r="P23" s="6"/>
-      <c r="Q23" s="6" t="s">
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="R23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6">
-        <v>0</v>
-      </c>
-      <c r="U23" s="6"/>
-    </row>
-    <row r="24" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6">
+        <v>0</v>
+      </c>
+      <c r="V23" s="6"/>
+    </row>
+    <row r="24" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
@@ -3388,21 +3436,22 @@
         <v>0</v>
       </c>
       <c r="P24" s="7"/>
-      <c r="Q24" s="7" t="s">
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="R24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7">
-        <v>0</v>
-      </c>
-      <c r="U24" s="7" t="s">
+      <c r="S24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7">
+        <v>0</v>
+      </c>
+      <c r="V24" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>48</v>
       </c>
@@ -3439,19 +3488,20 @@
         <v>0</v>
       </c>
       <c r="P25" s="7"/>
-      <c r="Q25" s="7" t="s">
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="R25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7">
-        <v>0</v>
-      </c>
-      <c r="U25" s="7"/>
-    </row>
-    <row r="26" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7">
+        <v>0</v>
+      </c>
+      <c r="V25" s="7"/>
+    </row>
+    <row r="26" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>99</v>
       </c>
@@ -3492,21 +3542,22 @@
         <v>0</v>
       </c>
       <c r="P26" s="7"/>
-      <c r="Q26" s="7" t="s">
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="R26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7">
-        <v>0</v>
-      </c>
-      <c r="U26" s="7" t="s">
+      <c r="S26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7">
+        <v>0</v>
+      </c>
+      <c r="V26" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>127</v>
       </c>
@@ -3549,23 +3600,24 @@
         <v>0</v>
       </c>
       <c r="P27" s="7"/>
-      <c r="Q27" s="7" t="s">
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="R27" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="S27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T27" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="T27" s="7">
-        <v>0</v>
-      </c>
-      <c r="U27" s="7" t="s">
+      <c r="U27" s="7">
+        <v>0</v>
+      </c>
+      <c r="V27" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>226</v>
       </c>
@@ -3606,21 +3658,22 @@
         <v>0</v>
       </c>
       <c r="P28" s="7"/>
-      <c r="Q28" s="7" t="s">
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="R28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7">
-        <v>0</v>
-      </c>
-      <c r="U28" s="7" t="s">
+      <c r="S28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7">
+        <v>0</v>
+      </c>
+      <c r="V28" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>276</v>
       </c>
@@ -3662,18 +3715,19 @@
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
-      <c r="R29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7">
-        <v>0</v>
-      </c>
-      <c r="U29" s="7" t="s">
+      <c r="R29" s="7"/>
+      <c r="S29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7">
+        <v>0</v>
+      </c>
+      <c r="V29" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>21</v>
       </c>
@@ -3716,23 +3770,24 @@
         <v>0</v>
       </c>
       <c r="P30" s="9"/>
-      <c r="Q30" s="9" t="s">
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="R30" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="S30" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="T30" s="9">
-        <v>0</v>
-      </c>
-      <c r="U30" s="9" t="s">
+      <c r="U30" s="9">
+        <v>0</v>
+      </c>
+      <c r="V30" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>32</v>
       </c>
@@ -3773,19 +3828,20 @@
         <v>0</v>
       </c>
       <c r="P31" s="10"/>
-      <c r="Q31" s="10" t="s">
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="R31" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10">
-        <v>0</v>
-      </c>
-      <c r="U31" s="10"/>
-    </row>
-    <row r="32" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S31" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10">
+        <v>0</v>
+      </c>
+      <c r="V31" s="10"/>
+    </row>
+    <row r="32" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>185</v>
       </c>
@@ -3822,19 +3878,20 @@
         <v>0</v>
       </c>
       <c r="P32" s="2"/>
-      <c r="Q32" s="2" t="s">
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="R32" s="2" t="s">
+      <c r="S32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2">
-        <v>0</v>
-      </c>
-      <c r="U32" s="2"/>
-    </row>
-    <row r="33" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T32" s="2"/>
+      <c r="U32" s="2">
+        <v>0</v>
+      </c>
+      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>81</v>
       </c>
@@ -3872,16 +3929,17 @@
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
-      <c r="R33" s="6" t="s">
+      <c r="R33" s="6"/>
+      <c r="S33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6">
-        <v>0</v>
-      </c>
-      <c r="U33" s="6"/>
-    </row>
-    <row r="34" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T33" s="6"/>
+      <c r="U33" s="6">
+        <v>0</v>
+      </c>
+      <c r="V33" s="6"/>
+    </row>
+    <row r="34" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>125</v>
       </c>
@@ -3916,21 +3974,22 @@
         <v>0</v>
       </c>
       <c r="P34" s="7"/>
-      <c r="Q34" s="7" t="s">
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="R34" s="7" t="s">
+      <c r="S34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7">
-        <v>0</v>
-      </c>
-      <c r="U34" s="7" t="s">
+      <c r="T34" s="7"/>
+      <c r="U34" s="7">
+        <v>0</v>
+      </c>
+      <c r="V34" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>281</v>
       </c>
@@ -3966,18 +4025,19 @@
       </c>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
-      <c r="R35" s="7" t="s">
+      <c r="R35" s="7"/>
+      <c r="S35" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7">
-        <v>0</v>
-      </c>
-      <c r="U35" s="7" t="s">
+      <c r="T35" s="7"/>
+      <c r="U35" s="7">
+        <v>0</v>
+      </c>
+      <c r="V35" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>83</v>
       </c>
@@ -4015,16 +4075,17 @@
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
-      <c r="R36" s="9" t="s">
+      <c r="R36" s="9"/>
+      <c r="S36" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9">
-        <v>0</v>
-      </c>
-      <c r="U36" s="9"/>
-    </row>
-    <row r="37" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T36" s="9"/>
+      <c r="U36" s="9">
+        <v>0</v>
+      </c>
+      <c r="V36" s="9"/>
+    </row>
+    <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>196</v>
       </c>
@@ -4062,16 +4123,17 @@
       </c>
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
-      <c r="R37" s="10" t="s">
+      <c r="R37" s="10"/>
+      <c r="S37" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10">
-        <v>0</v>
-      </c>
-      <c r="U37" s="10"/>
-    </row>
-    <row r="38" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T37" s="10"/>
+      <c r="U37" s="10">
+        <v>0</v>
+      </c>
+      <c r="V37" s="10"/>
+    </row>
+    <row r="38" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>291</v>
       </c>
@@ -4115,16 +4177,17 @@
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1">
-        <v>0</v>
-      </c>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R38" s="1"/>
+      <c r="S38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1">
+        <v>0</v>
+      </c>
+      <c r="V38" s="1"/>
+    </row>
+    <row r="39" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>240</v>
       </c>
@@ -4167,21 +4230,22 @@
         <v>0</v>
       </c>
       <c r="P39" s="5"/>
-      <c r="Q39" s="5" t="s">
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="R39" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5">
-        <v>0</v>
-      </c>
-      <c r="U39" s="5" t="s">
+      <c r="S39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5">
+        <v>0</v>
+      </c>
+      <c r="V39" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>246</v>
       </c>
@@ -4218,21 +4282,22 @@
         <v>0</v>
       </c>
       <c r="P40" s="5"/>
-      <c r="Q40" s="5" t="s">
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="R40" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5">
-        <v>0</v>
-      </c>
-      <c r="U40" s="5" t="s">
+      <c r="S40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5">
+        <v>0</v>
+      </c>
+      <c r="V40" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>260</v>
       </c>
@@ -4269,19 +4334,20 @@
         <v>0</v>
       </c>
       <c r="P41" s="5"/>
-      <c r="Q41" s="5" t="s">
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="R41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5">
-        <v>0</v>
-      </c>
-      <c r="U41" s="5"/>
-    </row>
-    <row r="42" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5">
+        <v>0</v>
+      </c>
+      <c r="V41" s="5"/>
+    </row>
+    <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>295</v>
       </c>
@@ -4322,21 +4388,22 @@
         <v>0</v>
       </c>
       <c r="P42" s="5"/>
-      <c r="Q42" s="5" t="s">
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="R42" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5">
-        <v>0</v>
-      </c>
-      <c r="U42" s="5" t="s">
+      <c r="S42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5">
+        <v>0</v>
+      </c>
+      <c r="V42" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>146</v>
       </c>
@@ -4373,17 +4440,17 @@
       <c r="O43" s="2">
         <v>0</v>
       </c>
-      <c r="Q43" s="2" t="s">
+      <c r="R43" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="R43" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T43" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>152</v>
       </c>
@@ -4420,17 +4487,17 @@
       <c r="O44" s="2">
         <v>0</v>
       </c>
-      <c r="Q44" s="2" t="s">
+      <c r="R44" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="R44" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T44" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U44" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>163</v>
       </c>
@@ -4464,17 +4531,17 @@
       <c r="O45" s="2">
         <v>0</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="R45" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="R45" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>179</v>
       </c>
@@ -4505,20 +4572,20 @@
       <c r="O46" s="2">
         <v>0</v>
       </c>
-      <c r="Q46" s="2" t="s">
+      <c r="R46" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="R46" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T46" s="2">
-        <v>0</v>
-      </c>
-      <c r="U46" s="2" t="s">
+      <c r="S46" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U46" s="2">
+        <v>0</v>
+      </c>
+      <c r="V46" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>251</v>
       </c>
@@ -4555,19 +4622,20 @@
         <v>0</v>
       </c>
       <c r="P47" s="6"/>
-      <c r="Q47" s="6" t="s">
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="R47" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6">
-        <v>0</v>
-      </c>
-      <c r="U47" s="6"/>
-    </row>
-    <row r="48" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S47" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T47" s="6"/>
+      <c r="U47" s="6">
+        <v>0</v>
+      </c>
+      <c r="V47" s="6"/>
+    </row>
+    <row r="48" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>62</v>
       </c>
@@ -4606,21 +4674,22 @@
         <v>0</v>
       </c>
       <c r="P48" s="7"/>
-      <c r="Q48" s="7" t="s">
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="R48" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S48" s="7"/>
-      <c r="T48" s="7">
-        <v>0</v>
-      </c>
-      <c r="U48" s="7" t="s">
+      <c r="S48" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7">
+        <v>0</v>
+      </c>
+      <c r="V48" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>87</v>
       </c>
@@ -4661,21 +4730,22 @@
         <v>0</v>
       </c>
       <c r="P49" s="7"/>
-      <c r="Q49" s="7" t="s">
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="R49" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S49" s="7"/>
-      <c r="T49" s="7">
-        <v>0</v>
-      </c>
-      <c r="U49" s="7" t="s">
+      <c r="S49" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7">
+        <v>0</v>
+      </c>
+      <c r="V49" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>122</v>
       </c>
@@ -4716,21 +4786,22 @@
         <v>0</v>
       </c>
       <c r="P50" s="7"/>
-      <c r="Q50" s="7" t="s">
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="R50" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S50" s="7"/>
-      <c r="T50" s="7">
-        <v>0</v>
-      </c>
-      <c r="U50" s="7" t="s">
+      <c r="S50" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7">
+        <v>0</v>
+      </c>
+      <c r="V50" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>233</v>
       </c>
@@ -4773,19 +4844,20 @@
         <v>0</v>
       </c>
       <c r="P51" s="7"/>
-      <c r="Q51" s="7" t="s">
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="R51" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S51" s="7"/>
-      <c r="T51" s="7">
-        <v>0</v>
-      </c>
-      <c r="U51" s="7"/>
-    </row>
-    <row r="52" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S51" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7">
+        <v>0</v>
+      </c>
+      <c r="V51" s="7"/>
+    </row>
+    <row r="52" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>228</v>
       </c>
@@ -4827,16 +4899,17 @@
       </c>
       <c r="P52" s="10"/>
       <c r="Q52" s="10"/>
-      <c r="R52" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S52" s="10"/>
-      <c r="T52" s="10">
-        <v>0</v>
-      </c>
-      <c r="U52" s="10"/>
-    </row>
-    <row r="53" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R52" s="10"/>
+      <c r="S52" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T52" s="10"/>
+      <c r="U52" s="10">
+        <v>0</v>
+      </c>
+      <c r="V52" s="10"/>
+    </row>
+    <row r="53" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>310</v>
       </c>
@@ -4875,19 +4948,20 @@
         <v>0</v>
       </c>
       <c r="P53" s="1"/>
-      <c r="Q53" s="1" t="s">
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="R53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1">
-        <v>0</v>
-      </c>
-      <c r="U53" s="1"/>
-    </row>
-    <row r="54" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1">
+        <v>0</v>
+      </c>
+      <c r="V53" s="1"/>
+    </row>
+    <row r="54" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>316</v>
       </c>
@@ -4924,19 +4998,20 @@
         <v>0</v>
       </c>
       <c r="P54" s="1"/>
-      <c r="Q54" s="1" t="s">
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="R54" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1">
-        <v>0</v>
-      </c>
-      <c r="U54" s="1"/>
-    </row>
-    <row r="55" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1">
+        <v>0</v>
+      </c>
+      <c r="V54" s="1"/>
+    </row>
+    <row r="55" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>358</v>
       </c>
@@ -4980,16 +5055,17 @@
       </c>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
-      <c r="R55" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1">
-        <v>0</v>
-      </c>
-      <c r="U55" s="1"/>
-    </row>
-    <row r="56" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R55" s="1"/>
+      <c r="S55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1">
+        <v>0</v>
+      </c>
+      <c r="V55" s="1"/>
+    </row>
+    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>365</v>
       </c>
@@ -5029,16 +5105,17 @@
         <v>367</v>
       </c>
       <c r="Q56" s="1"/>
-      <c r="R56" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1">
-        <v>0</v>
-      </c>
-      <c r="U56" s="1"/>
-    </row>
-    <row r="57" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R56" s="1"/>
+      <c r="S56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1">
+        <v>0</v>
+      </c>
+      <c r="V56" s="1"/>
+    </row>
+    <row r="57" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>381</v>
       </c>
@@ -5078,18 +5155,19 @@
       </c>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="R57" s="1"/>
       <c r="S57" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T57" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T57" s="1">
-        <v>0</v>
-      </c>
-      <c r="U57" s="1"/>
-    </row>
-    <row r="58" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U57" s="1">
+        <v>0</v>
+      </c>
+      <c r="V57" s="1"/>
+    </row>
+    <row r="58" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>307</v>
       </c>
@@ -5128,19 +5206,20 @@
         <v>0</v>
       </c>
       <c r="P58" s="5"/>
-      <c r="Q58" s="5" t="s">
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="R58" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S58" s="5"/>
-      <c r="T58" s="5">
-        <v>0</v>
-      </c>
-      <c r="U58" s="5"/>
-    </row>
-    <row r="59" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S58" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5">
+        <v>0</v>
+      </c>
+      <c r="V58" s="5"/>
+    </row>
+    <row r="59" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>342</v>
       </c>
@@ -5182,18 +5261,19 @@
       </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
-      <c r="R59" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S59" s="5"/>
-      <c r="T59" s="5">
-        <v>0</v>
-      </c>
-      <c r="U59" s="5" t="s">
+      <c r="R59" s="5"/>
+      <c r="S59" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5">
+        <v>0</v>
+      </c>
+      <c r="V59" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>77</v>
       </c>
@@ -5233,18 +5313,19 @@
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
-      <c r="R60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5">
-        <v>0</v>
-      </c>
-      <c r="U60" s="5" t="s">
+      <c r="R60" s="5"/>
+      <c r="S60" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T60" s="5"/>
+      <c r="U60" s="5">
+        <v>0</v>
+      </c>
+      <c r="V60" s="5" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>356</v>
       </c>
@@ -5286,18 +5367,19 @@
       </c>
       <c r="P61" s="5"/>
       <c r="Q61" s="5"/>
-      <c r="R61" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S61" s="5"/>
-      <c r="T61" s="5">
-        <v>0</v>
-      </c>
-      <c r="U61" s="5" t="s">
+      <c r="R61" s="5"/>
+      <c r="S61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5">
+        <v>0</v>
+      </c>
+      <c r="V61" s="5" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="62" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>319</v>
       </c>
@@ -5331,14 +5413,14 @@
       <c r="O62" s="9">
         <v>0</v>
       </c>
-      <c r="R62" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="T62" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S62" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="U62" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>320</v>
       </c>
@@ -5369,17 +5451,17 @@
       <c r="O63" s="6">
         <v>0</v>
       </c>
-      <c r="Q63" s="6" t="s">
+      <c r="R63" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="R63" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S63" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>335</v>
       </c>
@@ -5410,14 +5492,14 @@
       <c r="O64" s="6">
         <v>0</v>
       </c>
-      <c r="R64" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T64" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S64" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>337</v>
       </c>
@@ -5448,14 +5530,14 @@
       <c r="O65" s="6">
         <v>0</v>
       </c>
-      <c r="R65" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T65" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S65" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>339</v>
       </c>
@@ -5486,14 +5568,14 @@
       <c r="O66" s="6">
         <v>0</v>
       </c>
-      <c r="R66" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T66" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S66" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>350</v>
       </c>
@@ -5530,20 +5612,20 @@
       <c r="O67" s="6">
         <v>1</v>
       </c>
-      <c r="Q67" s="6" t="s">
+      <c r="R67" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="R67" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T67" s="6">
-        <v>0</v>
-      </c>
-      <c r="U67" s="6" t="s">
+      <c r="S67" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U67" s="6">
+        <v>0</v>
+      </c>
+      <c r="V67" s="6" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="68" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>353</v>
       </c>
@@ -5580,20 +5662,20 @@
       <c r="O68" s="6">
         <v>1</v>
       </c>
-      <c r="Q68" s="6" t="s">
+      <c r="R68" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="R68" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="T68" s="6">
-        <v>1</v>
-      </c>
-      <c r="U68" s="6" t="s">
+      <c r="S68" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U68" s="6">
+        <v>1</v>
+      </c>
+      <c r="V68" s="6" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>313</v>
       </c>
@@ -5632,19 +5714,20 @@
         <v>0</v>
       </c>
       <c r="P69" s="8"/>
-      <c r="Q69" s="8" t="s">
+      <c r="Q69" s="8"/>
+      <c r="R69" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="R69" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S69" s="8"/>
-      <c r="T69" s="8">
-        <v>0</v>
-      </c>
-      <c r="U69" s="8"/>
-    </row>
-    <row r="70" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T69" s="8"/>
+      <c r="U69" s="8">
+        <v>0</v>
+      </c>
+      <c r="V69" s="8"/>
+    </row>
+    <row r="70" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>333</v>
       </c>
@@ -5682,16 +5765,17 @@
       </c>
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
-      <c r="R70" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S70" s="8"/>
-      <c r="T70" s="8">
-        <v>0</v>
-      </c>
-      <c r="U70" s="8"/>
-    </row>
-    <row r="71" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R70" s="8"/>
+      <c r="S70" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T70" s="8"/>
+      <c r="U70" s="8">
+        <v>0</v>
+      </c>
+      <c r="V70" s="8"/>
+    </row>
+    <row r="71" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>39</v>
       </c>
@@ -5728,21 +5812,22 @@
         <v>0</v>
       </c>
       <c r="P71" s="7"/>
-      <c r="Q71" s="7" t="s">
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="R71" s="7" t="s">
+      <c r="S71" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="S71" s="7"/>
-      <c r="T71" s="7">
-        <v>0</v>
-      </c>
-      <c r="U71" s="7" t="s">
+      <c r="T71" s="7"/>
+      <c r="U71" s="7">
+        <v>0</v>
+      </c>
+      <c r="V71" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>224</v>
       </c>
@@ -5783,19 +5868,20 @@
         <v>0</v>
       </c>
       <c r="P72" s="1"/>
-      <c r="Q72" s="1" t="s">
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="R72" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S72" s="1"/>
-      <c r="T72" s="1">
-        <v>0</v>
-      </c>
-      <c r="U72" s="1"/>
-    </row>
-    <row r="73" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1">
+        <v>0</v>
+      </c>
+      <c r="V72" s="1"/>
+    </row>
+    <row r="73" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>258</v>
       </c>
@@ -5836,19 +5922,20 @@
         <v>0</v>
       </c>
       <c r="P73" s="1"/>
-      <c r="Q73" s="1" t="s">
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="R73" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1">
-        <v>0</v>
-      </c>
-      <c r="U73" s="1"/>
-    </row>
-    <row r="74" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1">
+        <v>0</v>
+      </c>
+      <c r="V73" s="1"/>
+    </row>
+    <row r="74" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>64</v>
       </c>
@@ -5889,19 +5976,20 @@
         <v>0</v>
       </c>
       <c r="P74" s="5"/>
-      <c r="Q74" s="5" t="s">
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="R74" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5">
-        <v>0</v>
-      </c>
-      <c r="U74" s="5"/>
-    </row>
-    <row r="75" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S74" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5">
+        <v>0</v>
+      </c>
+      <c r="V74" s="5"/>
+    </row>
+    <row r="75" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>393</v>
       </c>
@@ -5942,19 +6030,20 @@
         <v>0</v>
       </c>
       <c r="P75" s="5"/>
-      <c r="Q75" s="5" t="s">
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="R75" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5">
-        <v>0</v>
-      </c>
-      <c r="U75" s="5"/>
-    </row>
-    <row r="76" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S75" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T75" s="5"/>
+      <c r="U75" s="5">
+        <v>0</v>
+      </c>
+      <c r="V75" s="5"/>
+    </row>
+    <row r="76" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>238</v>
       </c>
@@ -5995,21 +6084,22 @@
         <v>0</v>
       </c>
       <c r="P76" s="5"/>
-      <c r="Q76" s="5" t="s">
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="R76" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5">
-        <v>0</v>
-      </c>
-      <c r="U76" s="5" t="s">
+      <c r="S76" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T76" s="5"/>
+      <c r="U76" s="5">
+        <v>0</v>
+      </c>
+      <c r="V76" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>283</v>
       </c>
@@ -6051,16 +6141,17 @@
       </c>
       <c r="P77" s="5"/>
       <c r="Q77" s="5"/>
-      <c r="R77" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5">
-        <v>0</v>
-      </c>
-      <c r="U77" s="5"/>
-    </row>
-    <row r="78" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R77" s="5"/>
+      <c r="S77" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T77" s="5"/>
+      <c r="U77" s="5">
+        <v>0</v>
+      </c>
+      <c r="V77" s="5"/>
+    </row>
+    <row r="78" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>133</v>
       </c>
@@ -6097,21 +6188,22 @@
         <v>0</v>
       </c>
       <c r="P78" s="2"/>
-      <c r="Q78" s="2" t="s">
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="R78" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="S78" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T78" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="T78" s="2">
-        <v>0</v>
-      </c>
-      <c r="U78" s="2"/>
-    </row>
-    <row r="79" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U78" s="2">
+        <v>0</v>
+      </c>
+      <c r="V78" s="2"/>
+    </row>
+    <row r="79" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>139</v>
       </c>
@@ -6148,21 +6240,22 @@
         <v>0</v>
       </c>
       <c r="P79" s="2"/>
-      <c r="Q79" s="2" t="s">
+      <c r="Q79" s="2"/>
+      <c r="R79" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="R79" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S79" s="2"/>
-      <c r="T79" s="2">
-        <v>0</v>
-      </c>
-      <c r="U79" s="2" t="s">
+      <c r="S79" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T79" s="2"/>
+      <c r="U79" s="2">
+        <v>0</v>
+      </c>
+      <c r="V79" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>156</v>
       </c>
@@ -6205,21 +6298,22 @@
         <v>0</v>
       </c>
       <c r="P80" s="2"/>
-      <c r="Q80" s="2" t="s">
+      <c r="Q80" s="2"/>
+      <c r="R80" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="R80" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S80" s="2"/>
-      <c r="T80" s="2">
-        <v>0</v>
-      </c>
-      <c r="U80" s="2" t="s">
+      <c r="S80" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T80" s="2"/>
+      <c r="U80" s="2">
+        <v>0</v>
+      </c>
+      <c r="V80" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>166</v>
       </c>
@@ -6258,21 +6352,22 @@
         <v>0</v>
       </c>
       <c r="P81" s="2"/>
-      <c r="Q81" s="2" t="s">
+      <c r="Q81" s="2"/>
+      <c r="R81" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="R81" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S81" s="2"/>
-      <c r="T81" s="2">
-        <v>0</v>
-      </c>
-      <c r="U81" s="2" t="s">
+      <c r="S81" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T81" s="2"/>
+      <c r="U81" s="2">
+        <v>0</v>
+      </c>
+      <c r="V81" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="82" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>182</v>
       </c>
@@ -6315,19 +6410,20 @@
         <v>0</v>
       </c>
       <c r="P82" s="2"/>
-      <c r="Q82" s="2" t="s">
+      <c r="Q82" s="2"/>
+      <c r="R82" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="R82" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S82" s="2"/>
-      <c r="T82" s="2">
-        <v>0</v>
-      </c>
-      <c r="U82" s="2"/>
-    </row>
-    <row r="83" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S82" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T82" s="2"/>
+      <c r="U82" s="2">
+        <v>0</v>
+      </c>
+      <c r="V82" s="2"/>
+    </row>
+    <row r="83" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>268</v>
       </c>
@@ -6364,19 +6460,20 @@
         <v>0</v>
       </c>
       <c r="P83" s="6"/>
-      <c r="Q83" s="6" t="s">
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="R83" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S83" s="6"/>
-      <c r="T83" s="6">
-        <v>0</v>
-      </c>
-      <c r="U83" s="6"/>
-    </row>
-    <row r="84" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S83" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T83" s="6"/>
+      <c r="U83" s="6">
+        <v>0</v>
+      </c>
+      <c r="V83" s="6"/>
+    </row>
+    <row r="84" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>45</v>
       </c>
@@ -6413,20 +6510,20 @@
       <c r="O84" s="7">
         <v>0</v>
       </c>
-      <c r="Q84" s="7" t="s">
+      <c r="R84" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="R84" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T84" s="7">
-        <v>0</v>
-      </c>
-      <c r="U84" s="7" t="s">
+      <c r="S84" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U84" s="7">
+        <v>0</v>
+      </c>
+      <c r="V84" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>109</v>
       </c>
@@ -6457,17 +6554,17 @@
       <c r="O85" s="7">
         <v>0</v>
       </c>
-      <c r="Q85" s="7" t="s">
+      <c r="R85" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="R85" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T85" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S85" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U85" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>119</v>
       </c>
@@ -6504,17 +6601,17 @@
       <c r="O86" s="7">
         <v>0</v>
       </c>
-      <c r="Q86" s="7" t="s">
+      <c r="R86" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="R86" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T86" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S86" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U86" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>274</v>
       </c>
@@ -6551,17 +6648,17 @@
       <c r="O87" s="7">
         <v>0</v>
       </c>
-      <c r="R87" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T87" s="7">
-        <v>0</v>
-      </c>
-      <c r="U87" s="7" t="s">
+      <c r="S87" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U87" s="7">
+        <v>0</v>
+      </c>
+      <c r="V87" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>278</v>
       </c>
@@ -6592,20 +6689,20 @@
       <c r="O88" s="7">
         <v>0</v>
       </c>
-      <c r="Q88" s="7" t="s">
+      <c r="R88" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="R88" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="T88" s="7">
-        <v>0</v>
-      </c>
-      <c r="U88" s="7" t="s">
+      <c r="S88" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U88" s="7">
+        <v>0</v>
+      </c>
+      <c r="V88" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
         <v>218</v>
       </c>
@@ -6642,21 +6739,22 @@
         <v>0</v>
       </c>
       <c r="P89" s="8"/>
-      <c r="Q89" s="8" t="s">
+      <c r="Q89" s="8"/>
+      <c r="R89" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="R89" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S89" s="8"/>
-      <c r="T89" s="8">
-        <v>0</v>
-      </c>
-      <c r="U89" s="8" t="s">
+      <c r="S89" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T89" s="8"/>
+      <c r="U89" s="8">
+        <v>0</v>
+      </c>
+      <c r="V89" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="s">
         <v>284</v>
       </c>
@@ -6697,19 +6795,20 @@
         <v>0</v>
       </c>
       <c r="P90" s="8"/>
-      <c r="Q90" s="8" t="s">
+      <c r="Q90" s="8"/>
+      <c r="R90" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="R90" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S90" s="8"/>
-      <c r="T90" s="8">
-        <v>0</v>
-      </c>
-      <c r="U90" s="8"/>
-    </row>
-    <row r="91" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S90" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T90" s="8"/>
+      <c r="U90" s="8">
+        <v>0</v>
+      </c>
+      <c r="V90" s="8"/>
+    </row>
+    <row r="91" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="s">
         <v>287</v>
       </c>
@@ -6751,16 +6850,17 @@
       </c>
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
-      <c r="R91" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S91" s="8"/>
-      <c r="T91" s="8">
-        <v>0</v>
-      </c>
-      <c r="U91" s="8"/>
-    </row>
-    <row r="92" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R91" s="8"/>
+      <c r="S91" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T91" s="8"/>
+      <c r="U91" s="8">
+        <v>0</v>
+      </c>
+      <c r="V91" s="8"/>
+    </row>
+    <row r="92" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="s">
         <v>302</v>
       </c>
@@ -6802,16 +6902,17 @@
       </c>
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
-      <c r="R92" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S92" s="8"/>
-      <c r="T92" s="8">
-        <v>0</v>
-      </c>
-      <c r="U92" s="8"/>
-    </row>
-    <row r="93" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R92" s="8"/>
+      <c r="S92" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T92" s="8"/>
+      <c r="U92" s="8">
+        <v>0</v>
+      </c>
+      <c r="V92" s="8"/>
+    </row>
+    <row r="93" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>30</v>
       </c>
@@ -6852,19 +6953,20 @@
         <v>0</v>
       </c>
       <c r="P93" s="9"/>
-      <c r="Q93" s="9" t="s">
+      <c r="Q93" s="9"/>
+      <c r="R93" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="R93" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S93" s="9"/>
-      <c r="T93" s="9">
-        <v>0</v>
-      </c>
-      <c r="U93" s="9"/>
-    </row>
-    <row r="94" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S93" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T93" s="9"/>
+      <c r="U93" s="9">
+        <v>0</v>
+      </c>
+      <c r="V93" s="9"/>
+    </row>
+    <row r="94" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>85</v>
       </c>
@@ -6905,19 +7007,20 @@
         <v>0</v>
       </c>
       <c r="P94" s="9"/>
-      <c r="Q94" s="9" t="s">
+      <c r="Q94" s="9"/>
+      <c r="R94" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="R94" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S94" s="9"/>
-      <c r="T94" s="9">
-        <v>0</v>
-      </c>
-      <c r="U94" s="9"/>
-    </row>
-    <row r="95" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S94" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T94" s="9"/>
+      <c r="U94" s="9">
+        <v>0</v>
+      </c>
+      <c r="V94" s="9"/>
+    </row>
+    <row r="95" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="s">
         <v>201</v>
       </c>
@@ -6956,19 +7059,20 @@
         <v>0</v>
       </c>
       <c r="P95" s="10"/>
-      <c r="Q95" s="10" t="s">
+      <c r="Q95" s="10"/>
+      <c r="R95" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="R95" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S95" s="10"/>
-      <c r="T95" s="10">
-        <v>0</v>
-      </c>
-      <c r="U95" s="10"/>
-    </row>
-    <row r="96" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S95" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T95" s="10"/>
+      <c r="U95" s="10">
+        <v>0</v>
+      </c>
+      <c r="V95" s="10"/>
+    </row>
+    <row r="96" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
         <v>203</v>
       </c>
@@ -7009,19 +7113,20 @@
         <v>0</v>
       </c>
       <c r="P96" s="10"/>
-      <c r="Q96" s="10" t="s">
+      <c r="Q96" s="10"/>
+      <c r="R96" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="R96" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S96" s="10"/>
-      <c r="T96" s="10">
-        <v>0</v>
-      </c>
-      <c r="U96" s="10"/>
-    </row>
-    <row r="97" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S96" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T96" s="10"/>
+      <c r="U96" s="10">
+        <v>0</v>
+      </c>
+      <c r="V96" s="10"/>
+    </row>
+    <row r="97" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
         <v>289</v>
       </c>
@@ -7063,16 +7168,17 @@
       </c>
       <c r="P97" s="10"/>
       <c r="Q97" s="10"/>
-      <c r="R97" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S97" s="10"/>
-      <c r="T97" s="10">
-        <v>0</v>
-      </c>
-      <c r="U97" s="10"/>
-    </row>
-    <row r="98" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R97" s="10"/>
+      <c r="S97" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T97" s="10"/>
+      <c r="U97" s="10">
+        <v>0</v>
+      </c>
+      <c r="V97" s="10"/>
+    </row>
+    <row r="98" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -7113,21 +7219,22 @@
         <v>0</v>
       </c>
       <c r="P98" s="1"/>
-      <c r="Q98" s="1" t="s">
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="R98" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S98" s="1"/>
-      <c r="T98" s="1">
-        <v>0</v>
-      </c>
-      <c r="U98" s="1" t="s">
+      <c r="S98" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T98" s="1"/>
+      <c r="U98" s="1">
+        <v>0</v>
+      </c>
+      <c r="V98" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>57</v>
       </c>
@@ -7168,19 +7275,20 @@
         <v>0</v>
       </c>
       <c r="P99" s="5"/>
-      <c r="Q99" s="5" t="s">
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="R99" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S99" s="5"/>
-      <c r="T99" s="5">
-        <v>0</v>
-      </c>
-      <c r="U99" s="5"/>
-    </row>
-    <row r="100" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S99" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T99" s="5"/>
+      <c r="U99" s="5">
+        <v>0</v>
+      </c>
+      <c r="V99" s="5"/>
+    </row>
+    <row r="100" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>192</v>
       </c>
@@ -7217,21 +7325,22 @@
         <v>0</v>
       </c>
       <c r="P100" s="5"/>
-      <c r="Q100" s="5" t="s">
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="R100" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S100" s="5"/>
-      <c r="T100" s="5">
-        <v>0</v>
-      </c>
-      <c r="U100" s="5" t="s">
+      <c r="S100" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T100" s="5"/>
+      <c r="U100" s="5">
+        <v>0</v>
+      </c>
+      <c r="V100" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="101" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>292</v>
       </c>
@@ -7268,21 +7377,22 @@
         <v>0</v>
       </c>
       <c r="P101" s="5"/>
-      <c r="Q101" s="5" t="s">
+      <c r="Q101" s="5"/>
+      <c r="R101" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="R101" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S101" s="5"/>
-      <c r="T101" s="5">
-        <v>0</v>
-      </c>
-      <c r="U101" s="5" t="s">
+      <c r="S101" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T101" s="5"/>
+      <c r="U101" s="5">
+        <v>0</v>
+      </c>
+      <c r="V101" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="102" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>136</v>
       </c>
@@ -7323,21 +7433,22 @@
         <v>0</v>
       </c>
       <c r="P102" s="2"/>
-      <c r="Q102" s="2" t="s">
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="R102" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S102" s="2"/>
-      <c r="T102" s="2">
-        <v>0</v>
-      </c>
-      <c r="U102" s="2" t="s">
+      <c r="S102" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T102" s="2"/>
+      <c r="U102" s="2">
+        <v>0</v>
+      </c>
+      <c r="V102" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>169</v>
       </c>
@@ -7374,19 +7485,20 @@
         <v>0</v>
       </c>
       <c r="P103" s="2"/>
-      <c r="Q103" s="2" t="s">
+      <c r="Q103" s="2"/>
+      <c r="R103" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="R103" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S103" s="2"/>
-      <c r="T103" s="2">
-        <v>0</v>
-      </c>
-      <c r="U103" s="2"/>
-    </row>
-    <row r="104" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S103" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T103" s="2"/>
+      <c r="U103" s="2">
+        <v>0</v>
+      </c>
+      <c r="V103" s="2"/>
+    </row>
+    <row r="104" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>172</v>
       </c>
@@ -7425,19 +7537,20 @@
         <v>0</v>
       </c>
       <c r="P104" s="2"/>
-      <c r="Q104" s="2" t="s">
+      <c r="Q104" s="2"/>
+      <c r="R104" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="R104" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S104" s="2"/>
-      <c r="T104" s="2">
-        <v>0</v>
-      </c>
-      <c r="U104" s="2"/>
-    </row>
-    <row r="105" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S104" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T104" s="2"/>
+      <c r="U104" s="2">
+        <v>0</v>
+      </c>
+      <c r="V104" s="2"/>
+    </row>
+    <row r="105" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>69</v>
       </c>
@@ -7478,21 +7591,22 @@
         <v>0</v>
       </c>
       <c r="P105" s="6"/>
-      <c r="Q105" s="6" t="s">
+      <c r="Q105" s="6"/>
+      <c r="R105" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="R105" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S105" s="6"/>
-      <c r="T105" s="6">
-        <v>0</v>
-      </c>
-      <c r="U105" s="6" t="s">
+      <c r="S105" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T105" s="6"/>
+      <c r="U105" s="6">
+        <v>0</v>
+      </c>
+      <c r="V105" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>116</v>
       </c>
@@ -7531,19 +7645,20 @@
         <v>0</v>
       </c>
       <c r="P106" s="6"/>
-      <c r="Q106" s="6" t="s">
+      <c r="Q106" s="6"/>
+      <c r="R106" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="R106" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S106" s="6"/>
-      <c r="T106" s="6">
-        <v>0</v>
-      </c>
-      <c r="U106" s="6"/>
-    </row>
-    <row r="107" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S106" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T106" s="6"/>
+      <c r="U106" s="6">
+        <v>0</v>
+      </c>
+      <c r="V106" s="6"/>
+    </row>
+    <row r="107" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>106</v>
       </c>
@@ -7580,19 +7695,20 @@
         <v>0</v>
       </c>
       <c r="P107" s="7"/>
-      <c r="Q107" s="7" t="s">
+      <c r="Q107" s="7"/>
+      <c r="R107" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="R107" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S107" s="7"/>
-      <c r="T107" s="7">
-        <v>0</v>
-      </c>
-      <c r="U107" s="7"/>
-    </row>
-    <row r="108" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S107" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T107" s="7"/>
+      <c r="U107" s="7">
+        <v>0</v>
+      </c>
+      <c r="V107" s="7"/>
+    </row>
+    <row r="108" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>298</v>
       </c>
@@ -7633,19 +7749,20 @@
         <v>0</v>
       </c>
       <c r="P108" s="7"/>
-      <c r="Q108" s="7" t="s">
+      <c r="Q108" s="7"/>
+      <c r="R108" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="R108" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S108" s="7"/>
-      <c r="T108" s="7">
-        <v>0</v>
-      </c>
-      <c r="U108" s="7"/>
-    </row>
-    <row r="109" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S108" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T108" s="7"/>
+      <c r="U108" s="7">
+        <v>0</v>
+      </c>
+      <c r="V108" s="7"/>
+    </row>
+    <row r="109" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10" t="s">
         <v>304</v>
       </c>
@@ -7682,19 +7799,20 @@
         <v>0</v>
       </c>
       <c r="P109" s="10"/>
-      <c r="Q109" s="10" t="s">
+      <c r="Q109" s="10"/>
+      <c r="R109" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="R109" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S109" s="10"/>
-      <c r="T109" s="10">
-        <v>0</v>
-      </c>
-      <c r="U109" s="10"/>
-    </row>
-    <row r="110" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S109" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T109" s="10"/>
+      <c r="U109" s="10">
+        <v>0</v>
+      </c>
+      <c r="V109" s="10"/>
+    </row>
+    <row r="110" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>208</v>
       </c>
@@ -7735,19 +7853,20 @@
         <v>0</v>
       </c>
       <c r="P110" s="5"/>
-      <c r="Q110" s="5" t="s">
+      <c r="Q110" s="5"/>
+      <c r="R110" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="R110" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S110" s="5"/>
-      <c r="T110" s="5">
-        <v>0</v>
-      </c>
-      <c r="U110" s="5"/>
-    </row>
-    <row r="111" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S110" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T110" s="5"/>
+      <c r="U110" s="5">
+        <v>0</v>
+      </c>
+      <c r="V110" s="5"/>
+    </row>
+    <row r="111" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>230</v>
       </c>
@@ -7788,21 +7907,22 @@
         <v>0</v>
       </c>
       <c r="P111" s="5"/>
-      <c r="Q111" s="5" t="s">
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="R111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S111" s="5"/>
-      <c r="T111" s="5">
-        <v>0</v>
-      </c>
-      <c r="U111" s="5" t="s">
+      <c r="S111" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T111" s="5"/>
+      <c r="U111" s="5">
+        <v>0</v>
+      </c>
+      <c r="V111" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="112" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>243</v>
       </c>
@@ -7839,21 +7959,22 @@
         <v>0</v>
       </c>
       <c r="P112" s="5"/>
-      <c r="Q112" s="5" t="s">
+      <c r="Q112" s="5"/>
+      <c r="R112" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="R112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S112" s="5"/>
-      <c r="T112" s="5">
-        <v>0</v>
-      </c>
-      <c r="U112" s="5" t="s">
+      <c r="S112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T112" s="5"/>
+      <c r="U112" s="5">
+        <v>0</v>
+      </c>
+      <c r="V112" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>141</v>
       </c>
@@ -7890,21 +8011,24 @@
         <v>0</v>
       </c>
       <c r="P113" s="2"/>
-      <c r="Q113" s="2" t="s">
+      <c r="Q113" s="2">
+        <v>0</v>
+      </c>
+      <c r="R113" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="R113" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S113" s="2"/>
-      <c r="T113" s="2">
-        <v>0</v>
-      </c>
-      <c r="U113" s="2" t="s">
+      <c r="S113" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T113" s="2"/>
+      <c r="U113" s="2">
+        <v>0</v>
+      </c>
+      <c r="V113" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="114" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>143</v>
       </c>
@@ -7945,21 +8069,22 @@
         <v>0</v>
       </c>
       <c r="P114" s="2"/>
-      <c r="Q114" s="2" t="s">
+      <c r="Q114" s="2"/>
+      <c r="R114" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="R114" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S114" s="2"/>
-      <c r="T114" s="2">
-        <v>0</v>
-      </c>
-      <c r="U114" s="2" t="s">
+      <c r="S114" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T114" s="2"/>
+      <c r="U114" s="2">
+        <v>0</v>
+      </c>
+      <c r="V114" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="115" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -8000,19 +8125,20 @@
         <v>0</v>
       </c>
       <c r="P115" s="2"/>
-      <c r="Q115" s="2" t="s">
+      <c r="Q115" s="2"/>
+      <c r="R115" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R115" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S115" s="2"/>
-      <c r="T115" s="2">
-        <v>0</v>
-      </c>
-      <c r="U115" s="2"/>
-    </row>
-    <row r="116" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S115" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T115" s="2"/>
+      <c r="U115" s="2">
+        <v>0</v>
+      </c>
+      <c r="V115" s="2"/>
+    </row>
+    <row r="116" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>159</v>
       </c>
@@ -8051,21 +8177,22 @@
         <v>0</v>
       </c>
       <c r="P116" s="2"/>
-      <c r="Q116" s="2" t="s">
+      <c r="Q116" s="2"/>
+      <c r="R116" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="R116" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S116" s="2"/>
-      <c r="T116" s="2">
-        <v>0</v>
-      </c>
-      <c r="U116" s="2" t="s">
+      <c r="S116" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T116" s="2"/>
+      <c r="U116" s="2">
+        <v>0</v>
+      </c>
+      <c r="V116" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="117" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>175</v>
       </c>
@@ -8104,21 +8231,22 @@
         <v>0</v>
       </c>
       <c r="P117" s="2"/>
-      <c r="Q117" s="2" t="s">
+      <c r="Q117" s="2"/>
+      <c r="R117" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="R117" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S117" s="2"/>
-      <c r="T117" s="2">
-        <v>0</v>
-      </c>
-      <c r="U117" s="2" t="s">
+      <c r="S117" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T117" s="2"/>
+      <c r="U117" s="2">
+        <v>0</v>
+      </c>
+      <c r="V117" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="118" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>59</v>
       </c>
@@ -8161,21 +8289,22 @@
         <v>0</v>
       </c>
       <c r="P118" s="6"/>
-      <c r="Q118" s="6" t="s">
+      <c r="Q118" s="6"/>
+      <c r="R118" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="R118" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S118" s="6"/>
-      <c r="T118" s="6">
-        <v>0</v>
-      </c>
-      <c r="U118" s="6" t="s">
+      <c r="S118" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T118" s="6"/>
+      <c r="U118" s="6">
+        <v>0</v>
+      </c>
+      <c r="V118" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>91</v>
       </c>
@@ -8214,21 +8343,24 @@
         <v>0</v>
       </c>
       <c r="P119" s="7"/>
-      <c r="Q119" s="7" t="s">
+      <c r="Q119" s="7">
+        <v>0</v>
+      </c>
+      <c r="R119" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="R119" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S119" s="7"/>
-      <c r="T119" s="7">
-        <v>0</v>
-      </c>
-      <c r="U119" s="7" t="s">
+      <c r="S119" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T119" s="7"/>
+      <c r="U119" s="7">
+        <v>0</v>
+      </c>
+      <c r="V119" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="120" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>112</v>
       </c>
@@ -8265,19 +8397,20 @@
         <v>0</v>
       </c>
       <c r="P120" s="7"/>
-      <c r="Q120" s="7" t="s">
+      <c r="Q120" s="7"/>
+      <c r="R120" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="R120" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S120" s="7"/>
-      <c r="T120" s="7">
-        <v>0</v>
-      </c>
-      <c r="U120" s="7"/>
-    </row>
-    <row r="121" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S120" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T120" s="7"/>
+      <c r="U120" s="7">
+        <v>0</v>
+      </c>
+      <c r="V120" s="7"/>
+    </row>
+    <row r="121" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="8" t="s">
         <v>215</v>
       </c>
@@ -8314,19 +8447,20 @@
         <v>0</v>
       </c>
       <c r="P121" s="8"/>
-      <c r="Q121" s="8" t="s">
+      <c r="Q121" s="8"/>
+      <c r="R121" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="R121" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S121" s="8"/>
-      <c r="T121" s="8">
-        <v>0</v>
-      </c>
-      <c r="U121" s="8"/>
-    </row>
-    <row r="122" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S121" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T121" s="8"/>
+      <c r="U121" s="8">
+        <v>0</v>
+      </c>
+      <c r="V121" s="8"/>
+    </row>
+    <row r="122" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
         <v>72</v>
       </c>
@@ -8366,20 +8500,20 @@
       <c r="O122" s="10">
         <v>0</v>
       </c>
-      <c r="Q122" s="10" t="s">
+      <c r="R122" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="R122" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="T122" s="10">
-        <v>0</v>
-      </c>
-      <c r="U122" s="10" t="s">
+      <c r="S122" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="U122" s="10">
+        <v>0</v>
+      </c>
+      <c r="V122" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="123" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="s">
         <v>198</v>
       </c>
@@ -8410,17 +8544,17 @@
       <c r="O123" s="10">
         <v>0</v>
       </c>
-      <c r="Q123" s="10" t="s">
+      <c r="R123" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="R123" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="T123" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S123" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="U123" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
         <v>236</v>
       </c>
@@ -8460,17 +8594,17 @@
       <c r="O124" s="10">
         <v>0</v>
       </c>
-      <c r="Q124" s="10" t="s">
+      <c r="R124" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="R124" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="T124" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S124" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="U124" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
         <v>386</v>
       </c>
@@ -8504,14 +8638,14 @@
       <c r="O125" s="10">
         <v>0</v>
       </c>
-      <c r="R125" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="T125" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S125" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="U125" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>324</v>
       </c>
@@ -8552,19 +8686,20 @@
         <v>0</v>
       </c>
       <c r="P126" s="1"/>
-      <c r="Q126" s="1" t="s">
+      <c r="Q126" s="1"/>
+      <c r="R126" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="R126" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S126" s="1"/>
-      <c r="T126" s="1">
-        <v>0</v>
-      </c>
-      <c r="U126" s="1"/>
-    </row>
-    <row r="127" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S126" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T126" s="1"/>
+      <c r="U126" s="1">
+        <v>0</v>
+      </c>
+      <c r="V126" s="1"/>
+    </row>
+    <row r="127" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>383</v>
       </c>
@@ -8604,18 +8739,19 @@
       </c>
       <c r="P127" s="1"/>
       <c r="Q127" s="1"/>
-      <c r="R127" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="R127" s="1"/>
       <c r="S127" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T127" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="T127" s="1">
-        <v>0</v>
-      </c>
-      <c r="U127" s="1"/>
-    </row>
-    <row r="128" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U127" s="1">
+        <v>0</v>
+      </c>
+      <c r="V127" s="1"/>
+    </row>
+    <row r="128" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>348</v>
       </c>
@@ -8655,16 +8791,17 @@
       </c>
       <c r="P128" s="5"/>
       <c r="Q128" s="5"/>
-      <c r="R128" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S128" s="5"/>
-      <c r="T128" s="5">
-        <v>0</v>
-      </c>
-      <c r="U128" s="5"/>
-    </row>
-    <row r="129" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R128" s="5"/>
+      <c r="S128" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T128" s="5"/>
+      <c r="U128" s="5">
+        <v>0</v>
+      </c>
+      <c r="V128" s="5"/>
+    </row>
+    <row r="129" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
         <v>341</v>
       </c>
@@ -8704,16 +8841,17 @@
       </c>
       <c r="P129" s="8"/>
       <c r="Q129" s="8"/>
-      <c r="R129" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S129" s="8"/>
-      <c r="T129" s="8">
-        <v>0</v>
-      </c>
-      <c r="U129" s="8"/>
-    </row>
-    <row r="130" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R129" s="8"/>
+      <c r="S129" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T129" s="8"/>
+      <c r="U129" s="8">
+        <v>0</v>
+      </c>
+      <c r="V129" s="8"/>
+    </row>
+    <row r="130" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>255</v>
       </c>
@@ -8756,19 +8894,22 @@
       <c r="P130" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="Q130" s="6" t="s">
+      <c r="Q130" s="6">
+        <v>0</v>
+      </c>
+      <c r="R130" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="R130" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S130" s="6"/>
-      <c r="T130" s="6">
+      <c r="S130" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T130" s="6"/>
+      <c r="U130" s="6">
         <v>-1</v>
       </c>
-      <c r="U130" s="6"/>
-    </row>
-    <row r="131" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="V130" s="6"/>
+    </row>
+    <row r="131" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>282</v>
       </c>
@@ -8810,18 +8951,19 @@
       </c>
       <c r="P131" s="7"/>
       <c r="Q131" s="7"/>
-      <c r="R131" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S131" s="7"/>
-      <c r="T131" s="7">
-        <v>0</v>
-      </c>
-      <c r="U131" s="7" t="s">
+      <c r="R131" s="7"/>
+      <c r="S131" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T131" s="7"/>
+      <c r="U131" s="7">
+        <v>0</v>
+      </c>
+      <c r="V131" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>363</v>
       </c>
@@ -8863,16 +9005,17 @@
       </c>
       <c r="P132" s="1"/>
       <c r="Q132" s="1"/>
-      <c r="R132" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S132" s="1"/>
-      <c r="T132" s="1">
-        <v>0</v>
-      </c>
-      <c r="U132" s="1"/>
-    </row>
-    <row r="133" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R132" s="1"/>
+      <c r="S132" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T132" s="1"/>
+      <c r="U132" s="1">
+        <v>0</v>
+      </c>
+      <c r="V132" s="1"/>
+    </row>
+    <row r="133" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>360</v>
       </c>
@@ -8912,16 +9055,17 @@
       </c>
       <c r="P133" s="5"/>
       <c r="Q133" s="5"/>
-      <c r="R133" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S133" s="5"/>
-      <c r="T133" s="5">
-        <v>0</v>
-      </c>
-      <c r="U133" s="5"/>
-    </row>
-    <row r="134" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R133" s="5"/>
+      <c r="S133" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T133" s="5"/>
+      <c r="U133" s="5">
+        <v>0</v>
+      </c>
+      <c r="V133" s="5"/>
+    </row>
+    <row r="134" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="10" t="s">
         <v>388</v>
       </c>
@@ -8958,14 +9102,14 @@
       <c r="O134" s="10">
         <v>0</v>
       </c>
-      <c r="R134" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="T134" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S134" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="U134" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>401</v>
       </c>
@@ -9002,14 +9146,14 @@
       <c r="O135">
         <v>0</v>
       </c>
-      <c r="R135" t="s">
+      <c r="S135" t="s">
         <v>42</v>
       </c>
-      <c r="T135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>402</v>
       </c>
@@ -9046,14 +9190,14 @@
       <c r="O136">
         <v>0</v>
       </c>
-      <c r="R136" t="s">
+      <c r="S136" t="s">
         <v>42</v>
       </c>
-      <c r="T136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>403</v>
       </c>
@@ -9081,10 +9225,10 @@
       <c r="O137">
         <v>0</v>
       </c>
-      <c r="R137" t="s">
+      <c r="S137" t="s">
         <v>42</v>
       </c>
-      <c r="T137">
+      <c r="U137">
         <v>0</v>
       </c>
     </row>

</xml_diff>